<commit_message>
appended 8th standup log to sprint 8 standup doc
</commit_message>
<xml_diff>
--- a/project_journal/assets/s8_assets/flask_apis.xlsx
+++ b/project_journal/assets/s8_assets/flask_apis.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_journal\assets\s8_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E81B6F2-9452-4B72-8190-1B5761BBB7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5CDAC0-7B1C-4AD4-86EE-E461AD0F32D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C551EE5F-BC6E-4444-BA40-FE73DEA46AED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C551EE5F-BC6E-4444-BA40-FE73DEA46AED}"/>
   </bookViews>
   <sheets>
-    <sheet name="api_doc" sheetId="6" r:id="rId1"/>
-    <sheet name="Sheet5" sheetId="11" r:id="rId2"/>
+    <sheet name="api_doc" sheetId="11" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Method</t>
   </si>
@@ -69,145 +68,13 @@
     <t>Test to see if Flask is online and working</t>
   </si>
   <si>
-    <t>Query params only (both mandatory)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">200: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>{ "ok": true, "service": "flask", "version": "x.y.z", "now": "2025-08-23T17:02:00Z", "response_time_ms": 120 }</t>
-    </r>
-  </si>
-  <si>
     <t>/api/notion/health</t>
   </si>
   <si>
-    <t>Test to see if Notion is working</t>
-  </si>
-  <si>
     <t>/api/db/health</t>
   </si>
   <si>
-    <t>Test to see if Supabase (database) is working; queries both user auth and target database</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">200: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>{ "ok": true, "service": "supabase", "version": "postgrest-x.y", "now": "…Z", "response_time_ms": 143.2, "checks": { "auth": { "ok": true, "status_code": 200 }, "database": { "ok": true, "status_code": 200 } } }</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">503: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>{ "ok": false, "service": "supabase", "version": "postgrest-x.y", "now": "…Z", "response_time_ms": 312.9, "checks": { "auth": { "ok": false, "status_code": 401 }, "database": { "ok": true, "status_code": 200 } }, "error": { "code": "network_error", "message": "Supabase auth inaccessible", "details": "..." } }</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">503: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>{ "ok": false, "service": "supabase", "version": "postgrest-x.y", "now": "…Z", "response_time_ms": 300, "checks": { "auth": { "ok": true, "status_code": 200 }, "database": { "ok": false, "status_code": 404 } }, "error": { "code": "network_error", "message": "Supabase database inaccessible", "details": "..." } }</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">500: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>{ "ok": false, "service": "supabase", "version": "postgrest-x.y", "now": "…Z", "response_time_ms": 500, "error": { "code": "internal_error", "message": "Unexpected error", "details": "..." } }</t>
-    </r>
-  </si>
-  <si>
-    <t>Request statistical metrics filtering work records by start and end date (inclusive)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">200: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>{ "ok": true, "service": "supabase", "version": "postgrest-x.y", "num_records": 42, "now": "…Z", "response_time_ms": 220, "meta": { "params": { "start_date": "YYYY-MM-DD", "end_date": "YYYY-MM-DD" } }, "data": { "week": { … }, "day": { … } } }</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">500: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>{ "ok": false, "service": "flask", "version": "x.y.z", "now": "…Z", "response_time_ms": 120, "error": { "code": "internal_error", "message": "Flask internal error", "details": "..." } }</t>
-    </r>
-  </si>
-  <si>
     <t>/api/db/stats?start=YYYY-MM-DD&amp;end=YYYY-MM-DD</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">200: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>{ "ok": true, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 102, "checks": { "user": { "ok": true, "status_code": 200 }, "database": { "ok": true, "status_code": 200 } } }</t>
-    </r>
-  </si>
-  <si>
-    <t>503 (user down): { "ok": false, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 150, "error": { "code": "user_inaccessible", "message": "Notion user endpoint inaccessible", "details": { "checks": { "user": { "ok": false, "status_code": 401 }, "database": { "ok": true, "status_code": 200 } } } } }503 (db down): { "ok": false, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 150, "error": { "code": "database_inaccessible", "message": "Notion database unreachable", "details": { "checks": { "user": { "ok": true, "status_code": 200 }, "database": { "ok": false, "status_code": 404 } } } } }503 (both down): { "ok": false, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 150, "error": { "code": "service_inaccessible", "message": "Notion user and database inaccessible", "details": { "checks": { "user": { "ok": false, "status_code": 401 }, "database": { "ok": false, "status_code": 404 } } } } }503 (network): { "ok": false, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 150, "error": { "code": "network_error", "message": "Network/HTTP failure while contacting Notion", "details": "requests.exceptions.RequestException(...)" } }500: { "ok": false, "service": "notion", "version": "2022-06-28", "now": "…Z", "response_time_ms": 150, "error": { "code": "internal_error", "message": "Unexpected error", "details": "..." } }</t>
-  </si>
-  <si>
-    <t>503: { "ok": false, "service": "supabase", "now": "…Z", "response_time_ms": 150, "error": { "code": "service_inaccessible", "message": "Supabase network not available", "details": "..." } }500: { "ok": false, "service": "supabase", "now": "…Z", "response_time_ms": 150, "error": { "code": "internal_error", "message": "Unexpected error", "details": "..." } }</t>
   </si>
   <si>
     <r>
@@ -582,21 +449,15 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -677,17 +538,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -708,17 +558,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -729,19 +568,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -764,148 +590,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -917,7 +696,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1253,135 +1038,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E949B3-D332-473A-972F-8E2D1FB52D13}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.21875" customWidth="1"/>
-    <col min="6" max="6" width="105" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="29.4" thickBot="1">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="41.4" thickBot="1">
-      <c r="A2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="173.4" thickBot="1">
-      <c r="A3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="96.6" thickBot="1">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="81" thickBot="1">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C509528-A7B4-4B02-A13F-71671DE00752}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1394,143 +1055,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.4" thickBot="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.8" thickBot="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="44" t="s">
-        <v>26</v>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="58.2" thickBot="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="41" t="s">
+      <c r="B3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="45" t="s">
-        <v>34</v>
+      <c r="E3" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.8" thickBot="1">
-      <c r="A4" s="27"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="50" t="s">
-        <v>35</v>
+    <row r="4" spans="1:6" ht="43.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="26" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.8" thickBot="1">
-      <c r="A5" s="27"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="50" t="s">
-        <v>36</v>
+    <row r="5" spans="1:6" ht="43.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="27" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29.4" thickBot="1">
-      <c r="A6" s="30"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="46" t="s">
-        <v>37</v>
+      <c r="A6" s="7"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="19" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.8" customHeight="1" thickBot="1">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:6" ht="43.8" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="41" t="s">
+      <c r="B7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="50" t="s">
-        <v>38</v>
+      <c r="E7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29.4" thickBot="1">
-      <c r="A8" s="30"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="46" t="s">
-        <v>39</v>
+      <c r="A8" s="7"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="19" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="72.599999999999994" thickBot="1">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>40</v>
+      <c r="F9" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added submission button with styling, added standup 10 to sprint 8's log
</commit_message>
<xml_diff>
--- a/project_journal/assets/s8_assets/flask_apis.xlsx
+++ b/project_journal/assets/s8_assets/flask_apis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_journal\assets\s8_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5CDAC0-7B1C-4AD4-86EE-E461AD0F32D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0A24F3-D59D-46B7-B12B-97CEFDE11F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C551EE5F-BC6E-4444-BA40-FE73DEA46AED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Method</t>
   </si>
@@ -421,6 +421,108 @@
       </rPr>
       <t>{ "ok": false, "service": "supabase", "now": "…Z", "response_time_ms": 150, "error": { "code": "internal_error", "message": "DB stats request: unexpected error occured", "details": "…" } }</t>
     </r>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/api/notion/plans</t>
+  </si>
+  <si>
+    <t>/api/db/plans</t>
+  </si>
+  <si>
+    <t>Post plan data to Notion's database table for easy access</t>
+  </si>
+  <si>
+    <t>Post plan + submission data to Supabase to keep track of overall plan goals</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: { "ok": true, "service": "supabase", "now": "...Z", "response_time_ms": 220, "data_stored": { "submission_id": 56, "last_modified": "...Z", "creation_date": "...Z", "synced_with_notion": false } }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>503</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: { "ok": false, "service": "supabase", "now": "...Z", "response_time_ms": 300, "error": { "code": "service_inaccessible", message: "Posting plans to Supabase failed! Service not currently available...", "details": {...} }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>500:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> { "ok": false, "service": "supabase", "now": "…Z", "response_time_ms": 150, "error": { "code": "internal_error", "message": "Posting plans to Supabase failed because an unexpected error occured", "details": "…" } }</t>
+    </r>
+  </si>
+  <si>
+    <t>Query params only (id for the submission_id)</t>
+  </si>
+  <si>
+    <t>200: { "ok": true, "service": "supabase", "now": "...Z", "response_time_ms": 220}</t>
+  </si>
+  <si>
+    <t>/api/plan-submissions/:id/sync</t>
+  </si>
+  <si>
+    <t>/api/plan-submissions</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>201: { "ok": true, "service": ["supabase", "notion"], "now": "...Z", "response_time_ms": 220, "sync_status": "pending"|"resolved"|"error", "synced_with_notion": false/true, "data": { "plans": [{...}, {...}, ...], "plan_submission": {"creation_date": "9/14/2025", "last_modified": "...Z", "submission_id": 1234, "stats": {"day": {...}, "week": {...}, "date_range": "..."}, "feasibility": {'overall': 'good', 'count': {'good': 3, 'moderate': 2, 'poor': 2}} }}}</t>
   </si>
 </sst>
 </file>
@@ -449,15 +551,27 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -618,11 +732,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -630,9 +794,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -667,9 +828,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -704,6 +862,61 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,6 +924,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1039,162 +1257,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C509528-A7B4-4B02-A13F-71671DE00752}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
     <col min="6" max="6" width="92.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.4" thickBot="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.8" thickBot="1">
+    <row r="2" spans="1:6" ht="41.4" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="58.2" thickBot="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6" ht="54.6" thickBot="1">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="13"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="17"/>
+      <c r="D4" s="15"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="17"/>
+      <c r="D5" s="15"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="25" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29.4" thickBot="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="19" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="17" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.8" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="24" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29.4" thickBot="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="19" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="72.599999999999994" thickBot="1">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:6" ht="67.8" thickBot="1">
+      <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="27" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.2">
+      <c r="A10" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="34"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1">
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+    </row>
+    <row r="12" spans="1:6" ht="65.400000000000006" customHeight="1">
+      <c r="A12" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="40"/>
+      <c r="E12" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="58.2" thickBot="1">
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14" s="26"/>
+      <c r="E14" s="26"/>
+    </row>
+    <row r="15" spans="1:6" ht="129.6">
+      <c r="A15" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="E15" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="80.400000000000006" customHeight="1">
+      <c r="A16" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="29"/>
+    </row>
+    <row r="17" spans="1:3" ht="63.6" customHeight="1">
+      <c r="A17" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated mvs and other documentation, started working on flask routes for submitting to Notion
</commit_message>
<xml_diff>
--- a/project_journal/assets/s8_assets/flask_apis.xlsx
+++ b/project_journal/assets/s8_assets/flask_apis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_journal\assets\s8_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0A24F3-D59D-46B7-B12B-97CEFDE11F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADF4414-00FA-4662-B2C2-4C839A96B986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C551EE5F-BC6E-4444-BA40-FE73DEA46AED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Method</t>
   </si>
@@ -426,16 +426,7 @@
     <t>POST</t>
   </si>
   <si>
-    <t>/api/notion/plans</t>
-  </si>
-  <si>
-    <t>/api/db/plans</t>
-  </si>
-  <si>
-    <t>Post plan data to Notion's database table for easy access</t>
-  </si>
-  <si>
-    <t>Post plan + submission data to Supabase to keep track of overall plan goals</t>
+    <t>/api/plan-submissions</t>
   </si>
   <si>
     <r>
@@ -447,17 +438,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>200</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: { "ok": true, "service": "supabase", "now": "...Z", "response_time_ms": 220, "data_stored": { "submission_id": 56, "last_modified": "...Z", "creation_date": "...Z", "synced_with_notion": false } }</t>
+      <t>502</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: {"ok":false,"service":["supabase","notion"],"now":"2025-09-14T15:25:00Z","response_time_ms":410,"sync_status":"failed","synced_with_notion":false,"error":{"code":"notion_sync_failed","message":"Plan submission could not be synced to Notion.","details":{"upstream":"503 Service Unavailable"}},"plan_submission":{"submission_id":"sub_125","sync_attempts":1,"last_sync_error":{"type":"UpstreamError","summary":"Notion 503"},"created_at":"2025-09-14T15:25:00Z","last_modified":"2025-09-14T15:25:00Z"}}</t>
     </r>
   </si>
   <si>
@@ -470,17 +461,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>503</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: { "ok": false, "service": "supabase", "now": "...Z", "response_time_ms": 300, "error": { "code": "service_inaccessible", message: "Posting plans to Supabase failed! Service not currently available...", "details": {...} }</t>
+      <t>400</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: {"ok":false,"service":["supabase"],"now":"2025-09-14T15:23:20Z","response_time_ms":35,"sync_status":null,"synced_with_notion":false,"error":{"code":"BAD_REQUEST","message":"Invalid input.","details":{"errors":[{"field":"plans[0].name","reason":"Required"},{"field":"plans[1].time_estimation","reason":"Must be a positive integer"}]}},"plan_submission":null}</t>
     </r>
   </si>
   <si>
@@ -493,36 +484,64 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>500:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> { "ok": false, "service": "supabase", "now": "…Z", "response_time_ms": 150, "error": { "code": "internal_error", "message": "Posting plans to Supabase failed because an unexpected error occured", "details": "…" } }</t>
-    </r>
-  </si>
-  <si>
-    <t>Query params only (id for the submission_id)</t>
-  </si>
-  <si>
-    <t>200: { "ok": true, "service": "supabase", "now": "...Z", "response_time_ms": 220}</t>
-  </si>
-  <si>
-    <t>/api/plan-submissions/:id/sync</t>
-  </si>
-  <si>
-    <t>/api/plan-submissions</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>201: { "ok": true, "service": ["supabase", "notion"], "now": "...Z", "response_time_ms": 220, "sync_status": "pending"|"resolved"|"error", "synced_with_notion": false/true, "data": { "plans": [{...}, {...}, ...], "plan_submission": {"creation_date": "9/14/2025", "last_modified": "...Z", "submission_id": 1234, "stats": {"day": {...}, "week": {...}, "date_range": "..."}, "feasibility": {'overall': 'good', 'count': {'good': 3, 'moderate': 2, 'poor': 2}} }}}</t>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: {"ok":false,"service":["supabase"],"now":"2025-09-14T15:24:30Z","response_time_ms":18,"sync_status":null,"synced_with_notion":false,"error":{"code":"internal_error","message":"An unexpected error occurred while creating the plan submission.","details":"{...}" },"plan_submission":null}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>201</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: {"ok":true,"service":["supabase","notion"],"now":"2025-09-14T15:23:00Z","response_time_ms":220,"num_plans":15,"plan_submission":{"submission_id":"sub_123","sync_attempts":1,"synced_with_notion":true,"sync_status":"success","created_at":"2025-09-14T15:23:00Z","last_modified":"2025-09-14T15:23:00Z"}}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>201</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: {"ok":true,"service":["supabase"],"now":"2025-09-14T15:23:00Z","response_time_ms":120,"num_plans":15,"plan_submission":{"submission_id":"sub_124","sync_attempts":0,"synced_with_notion":false,"sync_status":"pending","created_at":"2025-09-14T15:23:00Z","last_modified":"2025-09-14T15:23:00Z"}}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -551,27 +570,15 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF7C80"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -759,34 +766,15 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -863,59 +851,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1257,18 +1215,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C509528-A7B4-4B02-A13F-71671DE00752}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
     <col min="3" max="3" width="19.5546875" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" customWidth="1"/>
     <col min="6" max="6" width="92.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1392,113 +1350,63 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="67.8" thickBot="1">
+    <row r="9" spans="1:6" ht="58.2" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.2">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:6" ht="100.8">
+      <c r="A10" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="86.4">
+      <c r="A11" s="27"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="34"/>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1">
-      <c r="A11" s="35"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-    </row>
-    <row r="12" spans="1:6" ht="65.400000000000006" customHeight="1">
-      <c r="A12" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="39" t="s">
+    <row r="12" spans="1:6" ht="63.6" customHeight="1" thickBot="1">
+      <c r="A12" s="28"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="58.2" thickBot="1">
-      <c r="A13" s="42"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14" s="26"/>
-      <c r="E14" s="26"/>
-    </row>
-    <row r="15" spans="1:6" ht="129.6">
-      <c r="A15" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="29"/>
-      <c r="E15" s="26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="80.400000000000006" customHeight="1">
-      <c r="A16" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="29"/>
-    </row>
-    <row r="17" spans="1:3" ht="63.6" customHeight="1">
-      <c r="A17" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added standup log 4 for sprint 9
</commit_message>
<xml_diff>
--- a/project_journal/assets/s8_assets/flask_apis.xlsx
+++ b/project_journal/assets/s8_assets/flask_apis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_journal\assets\s8_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CB011C-6084-48A9-8FD9-3A074F3BDB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8113BB-862A-4F36-961E-995170AD3F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C551EE5F-BC6E-4444-BA40-FE73DEA46AED}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="150">
   <si>
     <t>Method</t>
   </si>
@@ -147,29 +147,6 @@
   </si>
   <si>
     <t>/api/plan-submissions</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>201:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{"ok":true,"service":["supabase"],"now":"2025-09-14T15:23:00Z","response_time_ms":120,"num_plans":15,"plan_submission":{"submission_id":123,"sync_attempts":0,"synced_with_notion":false,"sync_status":"pending","created_at":"2025-09-14T15:23:00Z","last_modified":"2025-09-14T15:23:00Z","filter_start_date":"2025-06-01","filter_end_date":"2025-06-30"}}</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1927,52 +1904,52 @@
     <row r="1" spans="6:11" ht="15" thickBot="1"/>
     <row r="2" spans="6:11" ht="15" thickBot="1">
       <c r="F2" s="85" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="86"/>
     </row>
     <row r="3" spans="6:11" ht="43.2" customHeight="1" thickBot="1">
       <c r="F3" s="83" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" s="84"/>
     </row>
     <row r="4" spans="6:11" ht="15" thickBot="1"/>
     <row r="5" spans="6:11" ht="15" thickBot="1">
       <c r="F5" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="H5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="I5" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="49" t="s">
+      <c r="J5" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="48" t="s">
-        <v>41</v>
-      </c>
       <c r="K5" s="62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="6:11">
       <c r="F6" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="H6" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="I6" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="60" t="s">
+      <c r="J6" s="59" t="s">
         <v>45</v>
-      </c>
-      <c r="J6" s="59" t="s">
-        <v>46</v>
       </c>
       <c r="K6" s="61" t="str">
         <f>"true"</f>
@@ -1981,59 +1958,59 @@
     </row>
     <row r="7" spans="6:11">
       <c r="F7" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="50" t="s">
+      <c r="I7" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="50" t="s">
+      <c r="K7" s="56" t="s">
         <v>49</v>
-      </c>
-      <c r="K7" s="56" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="8" spans="6:11" ht="28.8">
       <c r="F8" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="50" t="s">
+      <c r="I8" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="50" t="s">
-        <v>53</v>
-      </c>
       <c r="K8" s="56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="6:11" ht="15" thickBot="1">
       <c r="F9" s="63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="63" t="s">
+      <c r="I9" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="63" t="s">
         <v>56</v>
-      </c>
-      <c r="I9" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="63" t="s">
-        <v>57</v>
       </c>
       <c r="K9" s="65">
         <v>220</v>
@@ -2049,39 +2026,39 @@
     </row>
     <row r="11" spans="6:11" ht="28.8">
       <c r="F11" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="60" t="s">
+      <c r="H11" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="I11" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="J11" s="59" t="s">
-        <v>61</v>
-      </c>
       <c r="K11" s="61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="6:11" ht="29.4" thickBot="1">
       <c r="F12" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="64" t="s">
-        <v>63</v>
-      </c>
       <c r="H12" s="63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="64" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J12" s="63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K12" s="65">
         <v>1</v>
@@ -2097,19 +2074,19 @@
     </row>
     <row r="14" spans="6:11">
       <c r="F14" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="70" t="s">
+      <c r="H14" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="69" t="s">
         <v>65</v>
-      </c>
-      <c r="H14" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="J14" s="69" t="s">
-        <v>66</v>
       </c>
       <c r="K14" s="61">
         <v>42</v>
@@ -2117,42 +2094,42 @@
     </row>
     <row r="15" spans="6:11" ht="28.8">
       <c r="F15" s="51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="51" t="s">
+      <c r="I15" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="I15" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J15" s="51" t="s">
+      <c r="K15" s="56" t="s">
         <v>69</v>
-      </c>
-      <c r="K15" s="56" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" spans="6:11" ht="15" thickBot="1">
       <c r="F16" s="73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16" s="74" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="I16" s="74" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="73" t="s">
+      <c r="K16" s="65" t="s">
         <v>72</v>
-      </c>
-      <c r="K16" s="65" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="6:11" ht="15" thickBot="1">
@@ -2165,22 +2142,22 @@
     </row>
     <row r="18" spans="6:11" ht="29.4" thickBot="1">
       <c r="F18" s="75" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="76" t="s">
+      <c r="H18" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18" s="75" t="s">
+      <c r="K18" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="K18" s="77" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="6:11" ht="15" thickBot="1">
@@ -2193,22 +2170,22 @@
     </row>
     <row r="20" spans="6:11" ht="43.8" thickBot="1">
       <c r="F20" s="75" t="s">
+        <v>135</v>
+      </c>
+      <c r="G20" s="76" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" s="75" t="s">
+        <v>137</v>
+      </c>
+      <c r="I20" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="G20" s="76" t="s">
-        <v>115</v>
-      </c>
-      <c r="H20" s="75" t="s">
+      <c r="K20" s="77" t="s">
         <v>138</v>
-      </c>
-      <c r="I20" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="K20" s="77" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="21" spans="6:11" ht="15" thickBot="1">
@@ -2221,22 +2198,22 @@
     </row>
     <row r="22" spans="6:11" ht="15" thickBot="1">
       <c r="F22" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="G22" s="76" t="s">
+      <c r="H22" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="H22" s="75" t="s">
+      <c r="I22" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="I22" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="J22" s="75" t="s">
+      <c r="K22" s="77" t="s">
         <v>77</v>
-      </c>
-      <c r="K22" s="77" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="23" spans="6:11" ht="15" thickBot="1">
@@ -2249,19 +2226,19 @@
     </row>
     <row r="24" spans="6:11">
       <c r="F24" s="69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G24" s="70" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" s="69" t="s">
         <v>95</v>
-      </c>
-      <c r="H24" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="J24" s="69" t="s">
-        <v>96</v>
       </c>
       <c r="K24" s="61">
         <v>123</v>
@@ -2269,19 +2246,19 @@
     </row>
     <row r="25" spans="6:11">
       <c r="F25" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" s="51" t="s">
         <v>97</v>
-      </c>
-      <c r="H25" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J25" s="51" t="s">
-        <v>98</v>
       </c>
       <c r="K25" s="56">
         <v>1</v>
@@ -2289,19 +2266,19 @@
     </row>
     <row r="26" spans="6:11">
       <c r="F26" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G26" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J26" s="51" t="s">
         <v>99</v>
-      </c>
-      <c r="H26" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J26" s="51" t="s">
-        <v>100</v>
       </c>
       <c r="K26" s="56" t="str">
         <f>"false"</f>
@@ -2310,102 +2287,102 @@
     </row>
     <row r="27" spans="6:11">
       <c r="F27" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G27" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="H27" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="I27" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J27" s="51" t="s">
+      <c r="K27" s="56" t="s">
         <v>102</v>
-      </c>
-      <c r="K27" s="56" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="28" spans="6:11" ht="28.8">
       <c r="F28" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G28" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="I28" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J28" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="H28" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="I28" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J28" s="51" t="s">
-        <v>105</v>
-      </c>
       <c r="K28" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="6:11" ht="28.8">
       <c r="F29" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G29" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J29" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="H29" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="I29" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J29" s="51" t="s">
-        <v>107</v>
-      </c>
       <c r="K29" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="6:11" ht="28.8">
       <c r="F30" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="51" t="s">
+      <c r="I30" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J30" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="I30" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J30" s="51" t="s">
-        <v>81</v>
-      </c>
       <c r="K30" s="57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="6:11" ht="29.4" thickBot="1">
       <c r="F31" s="73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G31" s="74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H31" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="J31" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="I31" s="74" t="s">
-        <v>45</v>
-      </c>
-      <c r="J31" s="73" t="s">
-        <v>81</v>
-      </c>
       <c r="K31" s="78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="6:11" ht="15" thickBot="1">
@@ -2418,62 +2395,62 @@
     </row>
     <row r="33" spans="6:11" ht="43.2">
       <c r="F33" s="69" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="G33" s="70" t="s">
+      <c r="H33" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="I33" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="J33" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="H33" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="I33" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="J33" s="69" t="s">
+      <c r="K33" s="61" t="s">
         <v>89</v>
-      </c>
-      <c r="K33" s="61" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="34" spans="6:11" ht="28.8">
       <c r="F34" s="51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G34" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="I34" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J34" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="H34" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="I34" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J34" s="51" t="s">
+      <c r="K34" s="56" t="s">
         <v>92</v>
-      </c>
-      <c r="K34" s="56" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="35" spans="6:11" ht="29.4" thickBot="1">
       <c r="F35" s="73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G35" s="74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H35" s="73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I35" s="74" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J35" s="73" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K35" s="79" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="6:11" ht="15" thickBot="1">
@@ -2486,19 +2463,19 @@
     </row>
     <row r="37" spans="6:11" ht="28.8">
       <c r="F37" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="70" t="s">
+        <v>147</v>
+      </c>
+      <c r="H37" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="I37" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="J37" s="69" t="s">
         <v>108</v>
-      </c>
-      <c r="G37" s="70" t="s">
-        <v>148</v>
-      </c>
-      <c r="H37" s="69" t="s">
-        <v>80</v>
-      </c>
-      <c r="I37" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="J37" s="69" t="s">
-        <v>109</v>
       </c>
       <c r="K37" s="80">
         <v>45809</v>
@@ -2506,19 +2483,19 @@
     </row>
     <row r="38" spans="6:11" ht="28.8">
       <c r="F38" s="51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G38" s="54" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H38" s="51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I38" s="54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J38" s="51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K38" s="57">
         <v>45838</v>
@@ -2526,82 +2503,82 @@
     </row>
     <row r="39" spans="6:11" ht="28.8">
       <c r="F39" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="G39" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="H39" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="I39" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J39" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="K39" s="56" t="s">
         <v>111</v>
-      </c>
-      <c r="G39" s="54" t="s">
-        <v>145</v>
-      </c>
-      <c r="H39" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="I39" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J39" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="K39" s="56" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="40" spans="6:11" ht="28.8">
       <c r="F40" s="51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G40" s="54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H40" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I40" s="54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J40" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="K40" s="56" t="s">
         <v>113</v>
-      </c>
-      <c r="K40" s="56" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="41" spans="6:11" ht="28.8">
       <c r="F41" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="G41" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="H41" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="I41" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J41" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="G41" s="54" t="s">
-        <v>144</v>
-      </c>
-      <c r="H41" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="I41" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J41" s="51" t="s">
-        <v>142</v>
-      </c>
       <c r="K41" s="56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="6:11" ht="43.8" thickBot="1">
       <c r="F42" s="52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G42" s="55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H42" s="52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I42" s="55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J42" s="52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K42" s="58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="6:11">
@@ -2621,7 +2598,7 @@
   <dimension ref="B1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F16" sqref="F16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2637,14 +2614,14 @@
     <row r="1" spans="2:7" ht="15" thickBot="1"/>
     <row r="2" spans="2:7" ht="15" thickBot="1">
       <c r="B2" s="93" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="94"/>
       <c r="D2" s="95"/>
     </row>
     <row r="3" spans="2:7" ht="34.799999999999997" customHeight="1" thickBot="1">
       <c r="B3" s="90" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="91"/>
       <c r="D3" s="92"/>
@@ -2664,10 +2641,10 @@
         <v>5</v>
       </c>
       <c r="F5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>21</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="43.8" thickBot="1">
@@ -2684,10 +2661,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="42" t="s">
         <v>117</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="58.2" thickBot="1">
@@ -2704,10 +2681,10 @@
         <v>6</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="43.2">
@@ -2717,7 +2694,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="41"/>
       <c r="G8" s="44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="57.6">
@@ -2727,7 +2704,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="41"/>
       <c r="G9" s="45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="29.4" thickBot="1">
@@ -2737,7 +2714,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="46"/>
       <c r="G10" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="43.8" customHeight="1">
@@ -2754,10 +2731,10 @@
         <v>6</v>
       </c>
       <c r="F11" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="44" t="s">
         <v>119</v>
-      </c>
-      <c r="G11" s="44" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="29.4" thickBot="1">
@@ -2767,7 +2744,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="46"/>
       <c r="G12" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="58.2" thickBot="1">
@@ -2784,10 +2761,10 @@
         <v>14</v>
       </c>
       <c r="F13" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="115.2">
@@ -2799,25 +2776,23 @@
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="87" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="100.8">
+    </row>
+    <row r="15" spans="2:7" ht="57.6">
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
       <c r="D15" s="29"/>
       <c r="E15" s="88"/>
-      <c r="F15" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="F15" s="21"/>
       <c r="G15" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="63.6" customHeight="1" thickBot="1">
@@ -2827,7 +2802,7 @@
       <c r="E16" s="89"/>
       <c r="F16" s="22"/>
       <c r="G16" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2858,23 +2833,23 @@
     <row r="1" spans="2:4" ht="15" thickBot="1"/>
     <row r="2" spans="2:4" ht="15" thickBot="1">
       <c r="B2" s="96" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="97"/>
     </row>
     <row r="3" spans="2:4" ht="29.4" customHeight="1" thickBot="1">
       <c r="B3" s="90" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="92"/>
     </row>
     <row r="4" spans="2:4" ht="15" thickBot="1"/>
     <row r="5" spans="2:4" ht="15" thickBot="1">
       <c r="B5" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="33"/>
     </row>
@@ -2883,7 +2858,7 @@
         <v>200</v>
       </c>
       <c r="C6" s="82" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="33"/>
     </row>
@@ -2892,7 +2867,7 @@
         <v>201</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="33"/>
     </row>
@@ -2901,7 +2876,7 @@
         <v>500</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="33"/>
     </row>
@@ -2910,7 +2885,7 @@
         <v>503</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="33"/>
     </row>
@@ -2919,7 +2894,7 @@
         <v>502</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="33"/>
     </row>
@@ -2928,7 +2903,7 @@
         <v>400</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="33"/>
     </row>

</xml_diff>